<commit_message>
excel bom file is added
</commit_message>
<xml_diff>
--- a/OSSI-1 COMMS/design file/OSSI-1 COMMS BOM.xlsx
+++ b/OSSI-1 COMMS/design file/OSSI-1 COMMS BOM.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="401">
   <si>
     <t>Part</t>
   </si>
@@ -1205,6 +1205,12 @@
   </si>
   <si>
     <t>M50-3200545</t>
+  </si>
+  <si>
+    <t>Mini right angle 10-pin JTAG for MSP430</t>
+  </si>
+  <si>
+    <t>Harwin Inc</t>
   </si>
   <si>
     <t>Unless noted othersie,_x000a_- Capacitors: GCM series from Murata / CGA series from TDK_x000a_- Resistors: ERJ 1% or 5% series from Panasonic Electronic Components_x000a__x000a_All all can be purchased from Digikey.com</t>
@@ -3501,6 +3507,9 @@
       <c r="G157">
         <v>742792010</v>
       </c>
+      <c t="s" r="H157">
+        <v>43</v>
+      </c>
     </row>
     <row r="158">
       <c t="s" r="A158">
@@ -3943,10 +3952,22 @@
       <c t="s" r="C189">
         <v>397</v>
       </c>
+      <c t="s" r="E189">
+        <v>398</v>
+      </c>
+      <c t="s" r="F189">
+        <v>399</v>
+      </c>
+      <c t="s" r="G189">
+        <v>397</v>
+      </c>
+      <c t="s" r="H189">
+        <v>43</v>
+      </c>
     </row>
     <row customHeight="1" r="195" ht="64.5">
       <c t="s" s="1" r="A195">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c s="1" r="B195"/>
       <c s="1" r="C195"/>

</xml_diff>